<commit_message>
Added filepath error check
</commit_message>
<xml_diff>
--- a/testing/xlsx/main_output.xlsx
+++ b/testing/xlsx/main_output.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,11 +491,6 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>NUMBER OF PROGRAMME RUNS</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
           <t>SCRAP</t>
         </is>
       </c>
@@ -538,11 +533,6 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
           <t>9.26 %</t>
         </is>
       </c>
@@ -585,11 +575,6 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
           <t>34.02 %</t>
         </is>
       </c>
@@ -632,11 +617,6 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
           <t>83.52 %</t>
         </is>
       </c>
@@ -679,11 +659,6 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
           <t>30.07 %</t>
         </is>
       </c>
@@ -726,59 +701,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
           <t>0.95 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TC600L - TYPE: 1 (2535.0 x 1280.0 mm)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>/TRUMPF.NET/Workfiles/User1/test.LST</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1.4301-30</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2500 x 670 x 3 mm</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>39.70 kg</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>0 : 01 : 05 [h:min:s]</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>903.754 mm</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>49.03 %</t>
         </is>
       </c>
     </row>

</xml_diff>